<commit_message>
updated constraints to 0.2 mm diameter wire
</commit_message>
<xml_diff>
--- a/engineering-docs/betta-wire-engineering-calculations.xlsx
+++ b/engineering-docs/betta-wire-engineering-calculations.xlsx
@@ -232,7 +232,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,6 +257,12 @@
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
@@ -292,7 +298,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -345,15 +351,23 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,6 +381,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -552,20 +570,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R49"/>
+  <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M61" activeCellId="0" sqref="M61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="20.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.62"/>
@@ -993,10 +1011,10 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="n">
+      <c r="A16" s="12" t="n">
         <v>0.2</v>
       </c>
-      <c r="B16" s="10" t="str">
+      <c r="B16" s="12" t="str">
         <f aca="false">B2</f>
         <v>Aluminum </v>
       </c>
@@ -1016,11 +1034,11 @@
         <f aca="false">((3.14*((A16/2)^2))+(A16*F16*1000))*C16</f>
         <v>600.0942</v>
       </c>
-      <c r="H16" s="11" t="n">
+      <c r="H16" s="13" t="n">
         <f aca="false">((G16/(1000^3))*B3)*1000</f>
         <v>1.62025434</v>
       </c>
-      <c r="I16" s="11" t="n">
+      <c r="I16" s="13" t="n">
         <f aca="false">((H16/1000)*O16*(N16-R16)+((H16/1000)*P16)+((H16/1000)*Q16))/1000</f>
         <v>3.5669055952716</v>
       </c>
@@ -1207,19 +1225,19 @@
         <f aca="false">B2</f>
         <v>Aluminum </v>
       </c>
-      <c r="C19" s="13" t="n">
+      <c r="C19" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="D19" s="13" t="n">
+      <c r="D19" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="E19" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" s="13" t="n">
+      <c r="E19" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="14" t="n">
         <f aca="false">((3.14*((A19/2)^2))+(A19*F19*1000))*C19</f>
         <v>900.21195</v>
       </c>
@@ -1231,42 +1249,46 @@
         <f aca="false">((H19/1000)*O19*(N19-R19)+((H19/1000)*P19)+((H19/1000)*Q19))/1000</f>
         <v>5.35077833011111</v>
       </c>
-      <c r="J19" s="13" t="n">
+      <c r="J19" s="14" t="n">
         <f aca="false">((F19*1000)*60)/D19</f>
         <v>6000</v>
       </c>
-      <c r="K19" s="13" t="n">
+      <c r="K19" s="14" t="n">
         <f aca="false">(I19*1000)/J19</f>
         <v>0.891796388351851</v>
       </c>
-      <c r="L19" s="13" t="n">
+      <c r="L19" s="14" t="n">
         <f aca="false">B3</f>
         <v>2700</v>
       </c>
-      <c r="M19" s="13" t="n">
+      <c r="M19" s="14" t="n">
         <f aca="false">B4</f>
         <v>933</v>
       </c>
-      <c r="N19" s="13" t="n">
+      <c r="N19" s="14" t="n">
         <f aca="false">B5</f>
         <v>2740</v>
       </c>
-      <c r="O19" s="13" t="n">
+      <c r="O19" s="14" t="n">
         <f aca="false">B6</f>
         <v>897</v>
       </c>
-      <c r="P19" s="13" t="n">
+      <c r="P19" s="14" t="n">
         <f aca="false">B7</f>
         <v>397.5</v>
       </c>
-      <c r="Q19" s="13" t="n">
+      <c r="Q19" s="14" t="n">
         <f aca="false">B8</f>
         <v>10711</v>
       </c>
-      <c r="R19" s="13" t="n">
+      <c r="R19" s="14" t="n">
         <f aca="false">B9</f>
         <v>298.15</v>
       </c>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="n">
@@ -1691,10 +1713,10 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="n">
+      <c r="A30" s="12" t="n">
         <v>0.2</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C30" s="6" t="n">
@@ -1705,11 +1727,11 @@
         <f aca="false">3.14*((A30/2)^2)</f>
         <v>0.0314</v>
       </c>
-      <c r="E30" s="6" t="n">
+      <c r="E30" s="13" t="n">
         <f aca="false">F30*0.102</f>
         <v>2.72238</v>
       </c>
-      <c r="F30" s="6" t="n">
+      <c r="F30" s="13" t="n">
         <f aca="false">(C30*D30)</f>
         <v>26.69</v>
       </c>
@@ -1738,10 +1760,10 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="n">
+      <c r="A32" s="12" t="n">
         <v>0.3</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="6" t="n">
@@ -1752,42 +1774,42 @@
         <f aca="false">3.14*((A32/2)^2)</f>
         <v>0.07065</v>
       </c>
-      <c r="E32" s="6" t="n">
+      <c r="E32" s="13" t="n">
         <f aca="false">F32*0.102</f>
         <v>6.125355</v>
       </c>
-      <c r="F32" s="6" t="n">
+      <c r="F32" s="13" t="n">
         <f aca="false">(C32*D32)</f>
         <v>60.0525</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="n">
+      <c r="A33" s="16" t="n">
         <v>0.3</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="13" t="n">
+      <c r="C33" s="14" t="n">
         <v>950</v>
       </c>
-      <c r="D33" s="15" t="n">
+      <c r="D33" s="17" t="n">
         <f aca="false">3.14*((A33/2)^2)</f>
         <v>0.07065</v>
       </c>
-      <c r="E33" s="13" t="n">
+      <c r="E33" s="14" t="n">
         <f aca="false">F33*0.102</f>
         <v>6.845985</v>
       </c>
-      <c r="F33" s="13" t="n">
+      <c r="F33" s="14" t="n">
         <f aca="false">(C33*D33)</f>
         <v>67.1175</v>
       </c>
-      <c r="G33" s="16" t="s">
+      <c r="G33" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="n">
@@ -1837,120 +1859,120 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="2"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="19" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E38" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F38" s="18" t="s">
+      <c r="F38" s="20" t="s">
         <v>43</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H38" s="17" t="s">
+      <c r="H38" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I38" s="17" t="s">
+      <c r="I38" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="J38" s="17" t="s">
+      <c r="J38" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="K38" s="17" t="s">
+      <c r="K38" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L38" s="17" t="s">
+      <c r="L38" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="M38" s="17" t="s">
+      <c r="M38" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="N38" s="17" t="s">
+      <c r="N38" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="O38" s="17" t="s">
+      <c r="O38" s="19" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="13" t="n">
-        <v>8</v>
-      </c>
-      <c r="C39" s="13" t="n">
+      <c r="B39" s="21" t="n">
+        <v>4</v>
+      </c>
+      <c r="C39" s="21" t="n">
         <v>41</v>
       </c>
-      <c r="D39" s="13" t="n">
+      <c r="D39" s="21" t="n">
         <v>0.4</v>
       </c>
-      <c r="E39" s="13" t="n">
+      <c r="E39" s="21" t="n">
         <v>4.5</v>
       </c>
-      <c r="F39" s="13" t="n">
+      <c r="F39" s="21" t="n">
         <f aca="false">N39*B39</f>
-        <v>1.32</v>
-      </c>
-      <c r="G39" s="13" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G39" s="21" t="n">
         <f aca="false">F39*E39</f>
-        <v>5.94</v>
-      </c>
-      <c r="H39" s="13" t="s">
+        <v>2.97</v>
+      </c>
+      <c r="H39" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="I39" s="13" t="n">
+      <c r="I39" s="21" t="n">
         <v>16</v>
       </c>
-      <c r="J39" s="13" t="n">
+      <c r="J39" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="K39" s="13" t="n">
+      <c r="K39" s="21" t="n">
         <f aca="false">(I39*J39)/3.14159</f>
         <v>10.1859249615641</v>
       </c>
-      <c r="L39" s="13" t="n">
+      <c r="L39" s="21" t="n">
         <f aca="false">((D39*B39)/(K39/20))</f>
-        <v>6.28318</v>
-      </c>
-      <c r="M39" s="13" t="n">
+        <v>3.14158999999999</v>
+      </c>
+      <c r="M39" s="21" t="n">
         <f aca="false">L39/0.102</f>
-        <v>61.5998039215686</v>
-      </c>
-      <c r="N39" s="13" t="n">
+        <v>30.7999019607842</v>
+      </c>
+      <c r="N39" s="21" t="n">
         <v>0.165</v>
       </c>
-      <c r="O39" s="13" t="n">
+      <c r="O39" s="21" t="n">
         <f aca="false">3.14159*K39*(C39/60)</f>
         <v>21.8666666666667</v>
       </c>
@@ -2022,8 +2044,6 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="6"/>
-      <c r="C45" s="0"/>
-      <c r="D45" s="0"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -2033,14 +2053,9 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="6"/>
-      <c r="C46" s="0"/>
-      <c r="D46" s="0"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="0"/>
-      <c r="I46" s="0"/>
-      <c r="J46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="6"/>
@@ -2049,9 +2064,6 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="0"/>
-      <c r="I47" s="0"/>
-      <c r="J47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="6"/>

</xml_diff>